<commit_message>
Continue test on D2A
</commit_message>
<xml_diff>
--- a/Saved model/Saved Results.xlsx
+++ b/Saved model/Saved Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\albi2\Documents\GitHub\Variational-Autoencoder-for-EEG-analysis\Saved model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C0E822-3E20-42EE-8847-A7405287386D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC5A229A-4D3E-402E-A131-D8112B5B484E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -271,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -361,818 +361,25 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="164">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="84">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -2338,10 +1545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:R58"/>
+  <dimension ref="A2:T58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P58" sqref="P58"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N48" sqref="N48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2352,74 +1559,79 @@
     <col min="23" max="23" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
-      <c r="L4" s="31" t="s">
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="M4" s="31"/>
-      <c r="N4" s="31"/>
-      <c r="O4" s="31"/>
-      <c r="P4" s="31"/>
-      <c r="Q4" t="s">
+      <c r="M4" s="34"/>
+      <c r="N4" s="34"/>
+      <c r="O4" s="34"/>
+      <c r="P4" s="34"/>
+      <c r="Q4" s="35" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="R4" s="35"/>
+      <c r="S4" s="30"/>
+      <c r="T4" s="36"/>
+    </row>
+    <row r="5" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="32" t="s">
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="L5" s="32"/>
-      <c r="M5" s="32"/>
-      <c r="N5" s="32" t="s">
+      <c r="L5" s="33"/>
+      <c r="M5" s="33"/>
+      <c r="N5" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="O5" s="32"/>
-      <c r="P5" s="32"/>
-      <c r="Q5" s="32"/>
-    </row>
-    <row r="6" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O5" s="33"/>
+      <c r="P5" s="33"/>
+      <c r="Q5" s="33"/>
+      <c r="R5" s="33"/>
+      <c r="S5" s="33"/>
+    </row>
+    <row r="6" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>1</v>
       </c>
       <c r="B6" s="2">
-        <f t="shared" ref="B6:B14" si="0">AVERAGE(D6:S6)</f>
-        <v>0.82592573333333363</v>
+        <f>AVERAGE(D6:Z6)</f>
+        <v>0.82552062500000034</v>
       </c>
       <c r="C6" s="4">
-        <f t="shared" ref="C6:C14" si="1">MAX(D6:S6)</f>
+        <f>MAX(D6:Z6)</f>
         <v>0.85416700000000001</v>
       </c>
       <c r="D6" s="3">
@@ -2467,17 +1679,21 @@
       <c r="R6" s="27">
         <v>0.82291700000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S6" s="31">
+        <v>0.81944399999999995</v>
+      </c>
+      <c r="T6" s="31"/>
+    </row>
+    <row r="7" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>2</v>
       </c>
       <c r="B7" s="7">
-        <f t="shared" si="0"/>
-        <v>0.70046286666666679</v>
+        <f>AVERAGE(D7:Z7)</f>
+        <v>0.70225687500000011</v>
       </c>
       <c r="C7" s="9">
-        <f t="shared" si="1"/>
+        <f>MAX(D7:Z7)</f>
         <v>0.75</v>
       </c>
       <c r="D7" s="8">
@@ -2525,17 +1741,21 @@
       <c r="R7" s="27">
         <v>0.72569399999999995</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S7" s="31">
+        <v>0.72916700000000001</v>
+      </c>
+      <c r="T7" s="31"/>
+    </row>
+    <row r="8" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>3</v>
       </c>
       <c r="B8" s="7">
-        <f t="shared" si="0"/>
-        <v>0.87847226666666656</v>
+        <f t="shared" ref="B8:B14" si="0">AVERAGE(D8:Z8)</f>
+        <v>0.87782124999999989</v>
       </c>
       <c r="C8" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="C8:C14" si="1">MAX(D8:Z8)</f>
         <v>0.91666700000000001</v>
       </c>
       <c r="D8" s="8">
@@ -2583,14 +1803,18 @@
       <c r="R8" s="27">
         <v>0.86111099999999996</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S8" s="31">
+        <v>0.86805600000000005</v>
+      </c>
+      <c r="T8" s="31"/>
+    </row>
+    <row r="9" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>4</v>
       </c>
       <c r="B9" s="7">
         <f t="shared" si="0"/>
-        <v>0.7114583333333333</v>
+        <v>0.71321612499999998</v>
       </c>
       <c r="C9" s="9">
         <f t="shared" si="1"/>
@@ -2641,14 +1865,18 @@
       <c r="R9" s="27">
         <v>0.78645799999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S9" s="31">
+        <v>0.73958299999999999</v>
+      </c>
+      <c r="T9" s="31"/>
+    </row>
+    <row r="10" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>5</v>
       </c>
       <c r="B10" s="7">
         <f t="shared" si="0"/>
-        <v>0.76828713333333343</v>
+        <v>0.77322056250000015</v>
       </c>
       <c r="C10" s="9">
         <f t="shared" si="1"/>
@@ -2699,14 +1927,18 @@
       <c r="R10" s="27">
         <v>0.85416700000000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S10" s="31">
+        <v>0.84722200000000003</v>
+      </c>
+      <c r="T10" s="31"/>
+    </row>
+    <row r="11" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>6</v>
       </c>
       <c r="B11" s="7">
         <f t="shared" si="0"/>
-        <v>0.81712960000000001</v>
+        <v>0.81814231250000002</v>
       </c>
       <c r="C11" s="9">
         <f t="shared" si="1"/>
@@ -2757,14 +1989,18 @@
       <c r="R11" s="27">
         <v>0.85069399999999995</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S11" s="31">
+        <v>0.83333299999999999</v>
+      </c>
+      <c r="T11" s="31"/>
+    </row>
+    <row r="12" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7">
         <v>7</v>
       </c>
       <c r="B12" s="7">
         <f t="shared" si="0"/>
-        <v>0.83958340000000009</v>
+        <v>0.84136293750000002</v>
       </c>
       <c r="C12" s="9">
         <f t="shared" si="1"/>
@@ -2815,14 +2051,18 @@
       <c r="R12" s="27">
         <v>0.87847200000000003</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S12" s="31">
+        <v>0.86805600000000005</v>
+      </c>
+      <c r="T12" s="31"/>
+    </row>
+    <row r="13" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7">
         <v>8</v>
       </c>
       <c r="B13" s="7">
         <f t="shared" si="0"/>
-        <v>0.85486106666666672</v>
+        <v>0.85677081250000009</v>
       </c>
       <c r="C13" s="9">
         <f t="shared" si="1"/>
@@ -2873,14 +2113,18 @@
       <c r="R13" s="27">
         <v>0.875</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S13" s="31">
+        <v>0.88541700000000001</v>
+      </c>
+      <c r="T13" s="31"/>
+    </row>
+    <row r="14" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11">
         <v>9</v>
       </c>
       <c r="B14" s="7">
         <f t="shared" si="0"/>
-        <v>0.89189813333333334</v>
+        <v>0.89301212500000005</v>
       </c>
       <c r="C14" s="9">
         <f t="shared" si="1"/>
@@ -2931,12 +2175,16 @@
       <c r="R14" s="27">
         <v>0.91666700000000001</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S14" s="31">
+        <v>0.90972200000000003</v>
+      </c>
+      <c r="T14" s="31"/>
+    </row>
+    <row r="15" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8"/>
       <c r="B15" s="13">
         <f t="shared" ref="B15:C15" si="2">AVERAGE(B6:B14)</f>
-        <v>0.80978650370370386</v>
+        <v>0.81125818055555543</v>
       </c>
       <c r="C15" s="15">
         <f t="shared" si="2"/>
@@ -2947,7 +2195,7 @@
         <v>0.77372688888888896</v>
       </c>
       <c r="E15" s="14">
-        <f t="shared" ref="E15:R15" si="3">AVERAGE(E6:E14)</f>
+        <f t="shared" ref="E15:S15" si="3">AVERAGE(E6:E14)</f>
         <v>0.7754631111111111</v>
       </c>
       <c r="F15" s="14">
@@ -3002,33 +2250,41 @@
         <f t="shared" si="3"/>
         <v>0.84124222222222234</v>
       </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S15" s="8">
+        <f t="shared" si="3"/>
+        <v>0.83333333333333348</v>
+      </c>
+      <c r="T15" s="8"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="30" t="s">
+      <c r="D17" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="30"/>
-      <c r="J17" s="30"/>
-      <c r="K17" s="30"/>
-      <c r="L17" s="31" t="s">
+      <c r="E17" s="35"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
+      <c r="K17" s="35"/>
+      <c r="L17" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="M17" s="31"/>
-      <c r="N17" s="31"/>
-      <c r="O17" s="31"/>
-      <c r="P17" s="31"/>
-      <c r="Q17" t="s">
+      <c r="M17" s="34"/>
+      <c r="N17" s="34"/>
+      <c r="O17" s="34"/>
+      <c r="P17" s="34"/>
+      <c r="Q17" s="35" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="R17" s="35"/>
+      <c r="S17" s="30"/>
+      <c r="T17" s="36"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="5" t="s">
         <v>2</v>
@@ -3036,37 +2292,39 @@
       <c r="C18" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="32" t="s">
+      <c r="D18" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="32"/>
-      <c r="J18" s="32"/>
-      <c r="K18" s="32" t="s">
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
+      <c r="K18" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="L18" s="32"/>
-      <c r="M18" s="32"/>
-      <c r="N18" s="32" t="s">
+      <c r="L18" s="33"/>
+      <c r="M18" s="33"/>
+      <c r="N18" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="O18" s="32"/>
-      <c r="P18" s="32"/>
-      <c r="Q18" s="32"/>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="O18" s="33"/>
+      <c r="P18" s="33"/>
+      <c r="Q18" s="33"/>
+      <c r="R18" s="33"/>
+      <c r="S18" s="33"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>1</v>
       </c>
       <c r="B19" s="2">
-        <f t="shared" ref="B19:B27" si="4">AVERAGE(D19:S19)</f>
-        <v>0.82222228148148147</v>
+        <f>AVERAGE(D19:Z19)</f>
+        <v>0.8224827013888889</v>
       </c>
       <c r="C19" s="4">
-        <f t="shared" ref="C19:C27" si="5">MAX(D19:S19)</f>
+        <f>MAX(D19:Z19)</f>
         <v>0.85416700000000001</v>
       </c>
       <c r="D19" s="8">
@@ -3114,17 +2372,20 @@
       <c r="R19">
         <v>0.85416700000000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S19">
+        <v>0.82638900000000004</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <v>2</v>
       </c>
       <c r="B20" s="7">
-        <f t="shared" si="4"/>
-        <v>0.70671296296296293</v>
+        <f>AVERAGE(D20:Z20)</f>
+        <v>0.71028646527777783</v>
       </c>
       <c r="C20" s="9">
-        <f t="shared" si="5"/>
+        <f>MAX(D20:Z20)</f>
         <v>0.79166666666666596</v>
       </c>
       <c r="D20" s="8">
@@ -3172,17 +2433,20 @@
       <c r="R20">
         <v>0.71180600000000005</v>
       </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S20">
+        <v>0.76388900000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <v>3</v>
       </c>
       <c r="B21" s="7">
-        <f t="shared" si="4"/>
-        <v>0.87523141481481459</v>
+        <f t="shared" ref="B21:B27" si="4">AVERAGE(D21:Z21)</f>
+        <v>0.87521695138888866</v>
       </c>
       <c r="C21" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="C21:C27" si="5">MAX(D21:Z21)</f>
         <v>0.92361099999999996</v>
       </c>
       <c r="D21" s="8">
@@ -3230,14 +2494,17 @@
       <c r="R21">
         <v>0.89583299999999999</v>
       </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S21">
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <v>4</v>
       </c>
       <c r="B22" s="7">
         <f t="shared" si="4"/>
-        <v>0.70555555555555549</v>
+        <v>0.70833333333333326</v>
       </c>
       <c r="C22" s="9">
         <f t="shared" si="5"/>
@@ -3288,18 +2555,21 @@
       <c r="R22">
         <v>0.78125</v>
       </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S22">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <v>5</v>
       </c>
       <c r="B23" s="7">
         <f t="shared" si="4"/>
-        <v>0.77685185925925937</v>
+        <v>0.78016493055555558</v>
       </c>
       <c r="C23" s="9">
         <f t="shared" si="5"/>
-        <v>0.82291700000000001</v>
+        <v>0.82986099999999996</v>
       </c>
       <c r="D23" s="8">
         <v>0.68055600000000005</v>
@@ -3346,14 +2616,17 @@
       <c r="R23">
         <v>0.82291700000000001</v>
       </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S23">
+        <v>0.82986099999999996</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <v>6</v>
       </c>
       <c r="B24" s="7">
         <f t="shared" si="4"/>
-        <v>0.81458327407407405</v>
+        <v>0.8144530694444444</v>
       </c>
       <c r="C24" s="9">
         <f t="shared" si="5"/>
@@ -3404,14 +2677,17 @@
       <c r="R24">
         <v>0.84027799999999997</v>
       </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S24">
+        <v>0.8125</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <v>7</v>
       </c>
       <c r="B25" s="7">
         <f t="shared" si="4"/>
-        <v>0.83912045925925915</v>
+        <v>0.84071186805555542</v>
       </c>
       <c r="C25" s="9">
         <f t="shared" si="5"/>
@@ -3462,14 +2738,17 @@
       <c r="R25">
         <v>0.87847200000000003</v>
       </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S25">
+        <v>0.86458299999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <v>8</v>
       </c>
       <c r="B26" s="7">
         <f t="shared" si="4"/>
-        <v>0.85277776296296293</v>
+        <v>0.85438365277777772</v>
       </c>
       <c r="C26" s="9">
         <f t="shared" si="5"/>
@@ -3520,14 +2799,17 @@
       <c r="R26">
         <v>0.89236099999999996</v>
       </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S26">
+        <v>0.87847200000000003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" s="10">
         <v>9</v>
       </c>
       <c r="B27" s="7">
         <f t="shared" si="4"/>
-        <v>0.89120362222222194</v>
+        <v>0.89149295833333309</v>
       </c>
       <c r="C27" s="9">
         <f t="shared" si="5"/>
@@ -3578,18 +2860,21 @@
       <c r="R27">
         <v>0.90625</v>
       </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S27">
+        <v>0.89583299999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B28" s="13">
         <f t="shared" ref="B28" si="6">AVERAGE(B19:B27)</f>
-        <v>0.80936213251028799</v>
+        <v>0.81083621450617271</v>
       </c>
       <c r="C28" s="15">
         <f t="shared" ref="C28" si="7">AVERAGE(C19:C27)</f>
-        <v>0.8651620864197529</v>
+        <v>0.86593364197530842</v>
       </c>
       <c r="D28" s="8">
         <f>AVERAGE(D19:D27)</f>
@@ -3612,7 +2897,7 @@
         <v>0.78703699999999999</v>
       </c>
       <c r="I28" s="8">
-        <f t="shared" ref="I28:R28" si="8">AVERAGE(I19:I27)</f>
+        <f t="shared" ref="I28:S28" si="8">AVERAGE(I19:I27)</f>
         <v>0.79706777777777771</v>
       </c>
       <c r="J28" s="8">
@@ -3651,77 +2936,86 @@
         <f t="shared" si="8"/>
         <v>0.84259266666666677</v>
       </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S28" s="8">
+        <f t="shared" si="8"/>
+        <v>0.83294744444444435</v>
+      </c>
+      <c r="T28" s="8"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="L29" s="26"/>
       <c r="M29" s="26"/>
       <c r="N29" s="26"/>
       <c r="O29" s="26"/>
       <c r="P29" s="26"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>0</v>
       </c>
-      <c r="D32" s="30" t="s">
+      <c r="D32" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="E32" s="30"/>
-      <c r="F32" s="30"/>
-      <c r="G32" s="30"/>
-      <c r="H32" s="30"/>
-      <c r="I32" s="30"/>
-      <c r="J32" s="30"/>
-      <c r="K32" s="30"/>
-      <c r="L32" s="31" t="s">
+      <c r="E32" s="35"/>
+      <c r="F32" s="35"/>
+      <c r="G32" s="35"/>
+      <c r="H32" s="35"/>
+      <c r="I32" s="35"/>
+      <c r="J32" s="35"/>
+      <c r="K32" s="35"/>
+      <c r="L32" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="M32" s="31"/>
-      <c r="N32" s="31"/>
-      <c r="O32" s="31"/>
-      <c r="P32" s="31"/>
-      <c r="Q32" t="s">
+      <c r="M32" s="34"/>
+      <c r="N32" s="34"/>
+      <c r="O32" s="34"/>
+      <c r="P32" s="34"/>
+      <c r="Q32" s="35" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="R32" s="35"/>
+      <c r="S32" s="35"/>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B33" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D33" s="32" t="s">
+      <c r="D33" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="E33" s="32"/>
-      <c r="F33" s="32"/>
-      <c r="G33" s="32"/>
-      <c r="H33" s="32"/>
-      <c r="I33" s="32"/>
-      <c r="J33" s="32"/>
-      <c r="K33" s="32" t="s">
+      <c r="E33" s="33"/>
+      <c r="F33" s="33"/>
+      <c r="G33" s="33"/>
+      <c r="H33" s="33"/>
+      <c r="I33" s="33"/>
+      <c r="J33" s="33"/>
+      <c r="K33" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="L33" s="32"/>
-      <c r="M33" s="32"/>
-      <c r="N33" s="32" t="s">
+      <c r="L33" s="33"/>
+      <c r="M33" s="33"/>
+      <c r="N33" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="O33" s="32"/>
-      <c r="P33" s="32"/>
-      <c r="Q33" s="32"/>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="O33" s="33"/>
+      <c r="P33" s="33"/>
+      <c r="Q33" s="33"/>
+      <c r="R33" s="33"/>
+      <c r="S33" s="33"/>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>1</v>
       </c>
       <c r="B34" s="17">
         <f>B6 * 100</f>
-        <v>82.592573333333362</v>
+        <v>82.552062500000034</v>
       </c>
       <c r="C34" s="18">
-        <f t="shared" ref="C34:K34" si="9">C6 * 100</f>
+        <f t="shared" ref="C34:J34" si="9">C6 * 100</f>
         <v>85.416700000000006</v>
       </c>
       <c r="D34" s="20">
@@ -3761,7 +3055,7 @@
         <v>84.722200000000001</v>
       </c>
       <c r="M34" s="20">
-        <f t="shared" ref="M34:R34" si="10">M6 * 100</f>
+        <f t="shared" ref="M34:S34" si="10">M6 * 100</f>
         <v>85.069400000000002</v>
       </c>
       <c r="N34" s="20">
@@ -3784,14 +3078,19 @@
         <f t="shared" si="10"/>
         <v>82.291700000000006</v>
       </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S34" s="20">
+        <f t="shared" si="10"/>
+        <v>81.944400000000002</v>
+      </c>
+      <c r="T34" s="20"/>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A35" s="6">
         <v>2</v>
       </c>
       <c r="B35" s="19">
         <f t="shared" ref="B35:L42" si="11">B7 * 100</f>
-        <v>70.046286666666674</v>
+        <v>70.225687500000006</v>
       </c>
       <c r="C35" s="21">
         <f t="shared" si="11"/>
@@ -3834,7 +3133,7 @@
         <v>70.833299999999994</v>
       </c>
       <c r="M35" s="20">
-        <f t="shared" ref="M35:R35" si="12">M7 * 100</f>
+        <f t="shared" ref="M35:S35" si="12">M7 * 100</f>
         <v>75</v>
       </c>
       <c r="N35" s="20">
@@ -3857,14 +3156,19 @@
         <f t="shared" si="12"/>
         <v>72.569400000000002</v>
       </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S35" s="20">
+        <f t="shared" si="12"/>
+        <v>72.916700000000006</v>
+      </c>
+      <c r="T35" s="20"/>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A36" s="6">
         <v>3</v>
       </c>
       <c r="B36" s="19">
         <f t="shared" si="11"/>
-        <v>87.847226666666657</v>
+        <v>87.782124999999994</v>
       </c>
       <c r="C36" s="21">
         <f t="shared" si="11"/>
@@ -3907,7 +3211,7 @@
         <v>90.277799999999999</v>
       </c>
       <c r="M36" s="20">
-        <f t="shared" ref="M36:R36" si="13">M8 * 100</f>
+        <f t="shared" ref="M36:S36" si="13">M8 * 100</f>
         <v>91.666700000000006</v>
       </c>
       <c r="N36" s="20">
@@ -3930,14 +3234,19 @@
         <f t="shared" si="13"/>
         <v>86.111099999999993</v>
       </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S36" s="20">
+        <f t="shared" si="13"/>
+        <v>86.805599999999998</v>
+      </c>
+      <c r="T36" s="20"/>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A37" s="6">
         <v>4</v>
       </c>
       <c r="B37" s="19">
         <f t="shared" si="11"/>
-        <v>71.145833333333329</v>
+        <v>71.321612500000001</v>
       </c>
       <c r="C37" s="21">
         <f t="shared" si="11"/>
@@ -3980,7 +3289,7 @@
         <v>77.083299999999994</v>
       </c>
       <c r="M37" s="20">
-        <f t="shared" ref="M37:R37" si="14">M9 * 100</f>
+        <f t="shared" ref="M37:S37" si="14">M9 * 100</f>
         <v>76.5625</v>
       </c>
       <c r="N37" s="20">
@@ -4003,14 +3312,19 @@
         <f t="shared" si="14"/>
         <v>78.645799999999994</v>
       </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S37" s="20">
+        <f t="shared" si="14"/>
+        <v>73.958299999999994</v>
+      </c>
+      <c r="T37" s="20"/>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A38" s="6">
         <v>5</v>
       </c>
       <c r="B38" s="19">
         <f t="shared" si="11"/>
-        <v>76.82871333333334</v>
+        <v>77.322056250000017</v>
       </c>
       <c r="C38" s="21">
         <f t="shared" si="11"/>
@@ -4053,7 +3367,7 @@
         <v>77.777799999999999</v>
       </c>
       <c r="M38" s="20">
-        <f t="shared" ref="M38:R38" si="15">M10 * 100</f>
+        <f t="shared" ref="M38:S38" si="15">M10 * 100</f>
         <v>79.166700000000006</v>
       </c>
       <c r="N38" s="20">
@@ -4076,14 +3390,19 @@
         <f t="shared" si="15"/>
         <v>85.416700000000006</v>
       </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S38" s="20">
+        <f t="shared" si="15"/>
+        <v>84.722200000000001</v>
+      </c>
+      <c r="T38" s="20"/>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A39" s="6">
         <v>6</v>
       </c>
       <c r="B39" s="19">
         <f t="shared" si="11"/>
-        <v>81.712959999999995</v>
+        <v>81.814231250000006</v>
       </c>
       <c r="C39" s="21">
         <f t="shared" si="11"/>
@@ -4126,7 +3445,7 @@
         <v>82.638900000000007</v>
       </c>
       <c r="M39" s="20">
-        <f t="shared" ref="M39:R39" si="16">M11 * 100</f>
+        <f t="shared" ref="M39:S39" si="16">M11 * 100</f>
         <v>80.555599999999998</v>
       </c>
       <c r="N39" s="20">
@@ -4149,14 +3468,19 @@
         <f t="shared" si="16"/>
         <v>85.069400000000002</v>
       </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S39" s="20">
+        <f t="shared" si="16"/>
+        <v>83.333299999999994</v>
+      </c>
+      <c r="T39" s="20"/>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A40" s="6">
         <v>7</v>
       </c>
       <c r="B40" s="19">
         <f t="shared" si="11"/>
-        <v>83.958340000000007</v>
+        <v>84.136293750000007</v>
       </c>
       <c r="C40" s="21">
         <f t="shared" si="11"/>
@@ -4199,7 +3523,7 @@
         <v>84.375</v>
       </c>
       <c r="M40" s="20">
-        <f t="shared" ref="M40:R40" si="17">M12 * 100</f>
+        <f t="shared" ref="M40:S40" si="17">M12 * 100</f>
         <v>86.111099999999993</v>
       </c>
       <c r="N40" s="20">
@@ -4222,14 +3546,19 @@
         <f t="shared" si="17"/>
         <v>87.847200000000001</v>
       </c>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S40" s="20">
+        <f t="shared" si="17"/>
+        <v>86.805599999999998</v>
+      </c>
+      <c r="T40" s="20"/>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A41" s="6">
         <v>8</v>
       </c>
       <c r="B41" s="19">
         <f t="shared" si="11"/>
-        <v>85.486106666666672</v>
+        <v>85.677081250000015</v>
       </c>
       <c r="C41" s="21">
         <f t="shared" si="11"/>
@@ -4272,7 +3601,7 @@
         <v>86.111099999999993</v>
       </c>
       <c r="M41" s="20">
-        <f t="shared" ref="M41:R41" si="18">M13 * 100</f>
+        <f t="shared" ref="M41:S41" si="18">M13 * 100</f>
         <v>85.069400000000002</v>
       </c>
       <c r="N41" s="20">
@@ -4295,14 +3624,19 @@
         <f t="shared" si="18"/>
         <v>87.5</v>
       </c>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S41" s="20">
+        <f t="shared" si="18"/>
+        <v>88.541700000000006</v>
+      </c>
+      <c r="T41" s="20"/>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A42" s="10">
         <v>9</v>
       </c>
       <c r="B42" s="22">
         <f t="shared" si="11"/>
-        <v>89.189813333333333</v>
+        <v>89.301212500000005</v>
       </c>
       <c r="C42" s="23">
         <f t="shared" si="11"/>
@@ -4345,7 +3679,7 @@
         <v>89.236099999999993</v>
       </c>
       <c r="M42" s="20">
-        <f t="shared" ref="M42:R42" si="19">M14 * 100</f>
+        <f t="shared" ref="M42:S42" si="19">M14 * 100</f>
         <v>89.236099999999993</v>
       </c>
       <c r="N42" s="20">
@@ -4368,14 +3702,19 @@
         <f t="shared" si="19"/>
         <v>91.666700000000006</v>
       </c>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S42" s="20">
+        <f t="shared" si="19"/>
+        <v>90.972200000000001</v>
+      </c>
+      <c r="T42" s="20"/>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A43" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B43" s="24">
-        <f t="shared" ref="B43:R43" si="20">AVERAGE(B34:B42)</f>
-        <v>80.978650370370374</v>
+        <f t="shared" ref="B43:S43" si="20">AVERAGE(B34:B42)</f>
+        <v>81.12581805555557</v>
       </c>
       <c r="C43" s="25">
         <f t="shared" si="20"/>
@@ -4441,23 +3780,28 @@
         <f t="shared" si="20"/>
         <v>84.12422222222223</v>
       </c>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="D44" s="33"/>
-      <c r="E44" s="33"/>
-      <c r="F44" s="33"/>
-      <c r="G44" s="33"/>
-      <c r="H44" s="33"/>
-      <c r="I44" s="33"/>
-      <c r="J44" s="33"/>
-      <c r="K44" s="33"/>
-      <c r="L44" s="33"/>
-      <c r="M44" s="33"/>
-      <c r="N44" s="33"/>
-      <c r="O44" s="33"/>
-      <c r="P44" s="33"/>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S43" s="20">
+        <f t="shared" si="20"/>
+        <v>83.333333333333329</v>
+      </c>
+      <c r="T43" s="20"/>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="D44" s="32"/>
+      <c r="E44" s="32"/>
+      <c r="F44" s="32"/>
+      <c r="G44" s="32"/>
+      <c r="H44" s="32"/>
+      <c r="I44" s="32"/>
+      <c r="J44" s="32"/>
+      <c r="K44" s="32"/>
+      <c r="L44" s="32"/>
+      <c r="M44" s="32"/>
+      <c r="N44" s="32"/>
+      <c r="O44" s="32"/>
+      <c r="P44" s="32"/>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D45" s="28"/>
       <c r="E45" s="28"/>
       <c r="F45" s="28"/>
@@ -4472,66 +3816,70 @@
       <c r="O45" s="28"/>
       <c r="P45" s="28"/>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>1</v>
       </c>
-      <c r="D46" s="30" t="s">
+      <c r="D46" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="E46" s="30"/>
-      <c r="F46" s="30"/>
-      <c r="G46" s="30"/>
-      <c r="H46" s="30"/>
-      <c r="I46" s="30"/>
-      <c r="J46" s="30"/>
-      <c r="K46" s="30"/>
-      <c r="L46" s="31" t="s">
+      <c r="E46" s="35"/>
+      <c r="F46" s="35"/>
+      <c r="G46" s="35"/>
+      <c r="H46" s="35"/>
+      <c r="I46" s="35"/>
+      <c r="J46" s="35"/>
+      <c r="K46" s="35"/>
+      <c r="L46" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="M46" s="31"/>
-      <c r="N46" s="31"/>
-      <c r="O46" s="31"/>
-      <c r="P46" s="31"/>
-      <c r="Q46" t="s">
+      <c r="M46" s="34"/>
+      <c r="N46" s="34"/>
+      <c r="O46" s="34"/>
+      <c r="P46" s="34"/>
+      <c r="Q46" s="35" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="R46" s="35"/>
+      <c r="S46" s="35"/>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B47" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D47" s="32" t="s">
+      <c r="D47" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="E47" s="32"/>
-      <c r="F47" s="32"/>
-      <c r="G47" s="32"/>
-      <c r="H47" s="32"/>
-      <c r="I47" s="32"/>
-      <c r="J47" s="32"/>
-      <c r="K47" s="32" t="s">
+      <c r="E47" s="33"/>
+      <c r="F47" s="33"/>
+      <c r="G47" s="33"/>
+      <c r="H47" s="33"/>
+      <c r="I47" s="33"/>
+      <c r="J47" s="33"/>
+      <c r="K47" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="L47" s="32"/>
-      <c r="M47" s="32"/>
-      <c r="N47" s="32" t="s">
+      <c r="L47" s="33"/>
+      <c r="M47" s="33"/>
+      <c r="N47" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="O47" s="32"/>
-      <c r="P47" s="32"/>
-      <c r="Q47" s="32"/>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="O47" s="33"/>
+      <c r="P47" s="33"/>
+      <c r="Q47" s="33"/>
+      <c r="R47" s="33"/>
+      <c r="S47" s="33"/>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>1</v>
       </c>
       <c r="B48" s="17">
         <f>B19 * 100</f>
-        <v>82.222228148148147</v>
+        <v>82.248270138888884</v>
       </c>
       <c r="C48" s="18">
         <f t="shared" ref="C48:K48" si="21">C19 * 100</f>
@@ -4574,7 +3922,7 @@
         <v>85.416700000000006</v>
       </c>
       <c r="M48" s="20">
-        <f t="shared" ref="M48:R48" si="22">M19 * 100</f>
+        <f t="shared" ref="M48:S48" si="22">M19 * 100</f>
         <v>82.291700000000006</v>
       </c>
       <c r="N48" s="20">
@@ -4597,14 +3945,19 @@
         <f t="shared" si="22"/>
         <v>85.416700000000006</v>
       </c>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S48" s="20">
+        <f t="shared" si="22"/>
+        <v>82.638900000000007</v>
+      </c>
+      <c r="T48" s="20"/>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A49" s="6">
         <v>2</v>
       </c>
       <c r="B49" s="19">
         <f t="shared" ref="B49:L49" si="23">B20 * 100</f>
-        <v>70.671296296296291</v>
+        <v>71.028646527777781</v>
       </c>
       <c r="C49" s="21">
         <f t="shared" si="23"/>
@@ -4647,7 +4000,7 @@
         <v>69.791700000000006</v>
       </c>
       <c r="M49" s="20">
-        <f t="shared" ref="M49:R49" si="24">M20 * 100</f>
+        <f t="shared" ref="M49:S49" si="24">M20 * 100</f>
         <v>73.958299999999994</v>
       </c>
       <c r="N49" s="20">
@@ -4670,14 +4023,19 @@
         <f t="shared" si="24"/>
         <v>71.180599999999998</v>
       </c>
-    </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S49" s="20">
+        <f t="shared" si="24"/>
+        <v>76.388900000000007</v>
+      </c>
+      <c r="T49" s="20"/>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A50" s="6">
         <v>3</v>
       </c>
       <c r="B50" s="19">
         <f t="shared" ref="B50:L50" si="25">B21 * 100</f>
-        <v>87.52314148148146</v>
+        <v>87.521695138888873</v>
       </c>
       <c r="C50" s="21">
         <f t="shared" si="25"/>
@@ -4720,7 +4078,7 @@
         <v>88.888900000000007</v>
       </c>
       <c r="M50" s="20">
-        <f t="shared" ref="M50:R50" si="26">M21 * 100</f>
+        <f t="shared" ref="M50:S50" si="26">M21 * 100</f>
         <v>87.5</v>
       </c>
       <c r="N50" s="20">
@@ -4743,14 +4101,19 @@
         <f t="shared" si="26"/>
         <v>89.583299999999994</v>
       </c>
-    </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S50" s="20">
+        <f t="shared" si="26"/>
+        <v>87.5</v>
+      </c>
+      <c r="T50" s="20"/>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A51" s="6">
         <v>4</v>
       </c>
       <c r="B51" s="19">
         <f t="shared" ref="B51:L51" si="27">B22 * 100</f>
-        <v>70.555555555555543</v>
+        <v>70.833333333333329</v>
       </c>
       <c r="C51" s="21">
         <f t="shared" si="27"/>
@@ -4793,7 +4156,7 @@
         <v>75</v>
       </c>
       <c r="M51" s="20">
-        <f t="shared" ref="M51:R51" si="28">M22 * 100</f>
+        <f t="shared" ref="M51:S51" si="28">M22 * 100</f>
         <v>78.125</v>
       </c>
       <c r="N51" s="20">
@@ -4816,18 +4179,23 @@
         <f t="shared" si="28"/>
         <v>78.125</v>
       </c>
-    </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S51" s="20">
+        <f t="shared" si="28"/>
+        <v>75</v>
+      </c>
+      <c r="T51" s="20"/>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A52" s="6">
         <v>5</v>
       </c>
       <c r="B52" s="19">
         <f t="shared" ref="B52:L52" si="29">B23 * 100</f>
-        <v>77.685185925925936</v>
+        <v>78.016493055555557</v>
       </c>
       <c r="C52" s="21">
         <f t="shared" si="29"/>
-        <v>82.291700000000006</v>
+        <v>82.986099999999993</v>
       </c>
       <c r="D52" s="20">
         <f t="shared" si="29"/>
@@ -4866,7 +4234,7 @@
         <v>78.819400000000002</v>
       </c>
       <c r="M52" s="20">
-        <f t="shared" ref="M52:R52" si="30">M23 * 100</f>
+        <f t="shared" ref="M52:S52" si="30">M23 * 100</f>
         <v>82.291700000000006</v>
       </c>
       <c r="N52" s="20">
@@ -4889,14 +4257,19 @@
         <f t="shared" si="30"/>
         <v>82.291700000000006</v>
       </c>
-    </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S52" s="20">
+        <f t="shared" si="30"/>
+        <v>82.986099999999993</v>
+      </c>
+      <c r="T52" s="20"/>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A53" s="6">
         <v>6</v>
       </c>
       <c r="B53" s="19">
         <f t="shared" ref="B53:L53" si="31">B24 * 100</f>
-        <v>81.45832740740741</v>
+        <v>81.44530694444444</v>
       </c>
       <c r="C53" s="21">
         <f t="shared" si="31"/>
@@ -4939,7 +4312,7 @@
         <v>81.944400000000002</v>
       </c>
       <c r="M53" s="20">
-        <f t="shared" ref="M53:R53" si="32">M24 * 100</f>
+        <f t="shared" ref="M53:S53" si="32">M24 * 100</f>
         <v>81.597200000000001</v>
       </c>
       <c r="N53" s="20">
@@ -4962,14 +4335,19 @@
         <f t="shared" si="32"/>
         <v>84.027799999999999</v>
       </c>
-    </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S53" s="20">
+        <f t="shared" si="32"/>
+        <v>81.25</v>
+      </c>
+      <c r="T53" s="20"/>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A54" s="6">
         <v>7</v>
       </c>
       <c r="B54" s="19">
         <f t="shared" ref="B54:L54" si="33">B25 * 100</f>
-        <v>83.912045925925909</v>
+        <v>84.071186805555541</v>
       </c>
       <c r="C54" s="21">
         <f t="shared" si="33"/>
@@ -5012,7 +4390,7 @@
         <v>83.680599999999998</v>
       </c>
       <c r="M54" s="20">
-        <f t="shared" ref="M54:R54" si="34">M25 * 100</f>
+        <f t="shared" ref="M54:S54" si="34">M25 * 100</f>
         <v>83.680599999999998</v>
       </c>
       <c r="N54" s="20">
@@ -5035,14 +4413,19 @@
         <f t="shared" si="34"/>
         <v>87.847200000000001</v>
       </c>
-    </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S54" s="20">
+        <f t="shared" si="34"/>
+        <v>86.458299999999994</v>
+      </c>
+      <c r="T54" s="20"/>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A55" s="6">
         <v>8</v>
       </c>
       <c r="B55" s="19">
         <f t="shared" ref="B55:L55" si="35">B26 * 100</f>
-        <v>85.277776296296295</v>
+        <v>85.438365277777777</v>
       </c>
       <c r="C55" s="21">
         <f t="shared" si="35"/>
@@ -5085,7 +4468,7 @@
         <v>87.5</v>
       </c>
       <c r="M55" s="20">
-        <f t="shared" ref="M55:R55" si="36">M26 * 100</f>
+        <f t="shared" ref="M55:S55" si="36">M26 * 100</f>
         <v>83.333299999999994</v>
       </c>
       <c r="N55" s="20">
@@ -5108,14 +4491,19 @@
         <f t="shared" si="36"/>
         <v>89.236099999999993</v>
       </c>
-    </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S55" s="20">
+        <f t="shared" si="36"/>
+        <v>87.847200000000001</v>
+      </c>
+      <c r="T55" s="20"/>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A56" s="10">
         <v>9</v>
       </c>
       <c r="B56" s="22">
         <f t="shared" ref="B56:L56" si="37">B27 * 100</f>
-        <v>89.120362222222198</v>
+        <v>89.149295833333312</v>
       </c>
       <c r="C56" s="23">
         <f t="shared" si="37"/>
@@ -5158,7 +4546,7 @@
         <v>92.013900000000007</v>
       </c>
       <c r="M56" s="20">
-        <f t="shared" ref="M56:R56" si="38">M27 * 100</f>
+        <f t="shared" ref="M56:S56" si="38">M27 * 100</f>
         <v>89.583299999999994</v>
       </c>
       <c r="N56" s="20">
@@ -5181,18 +4569,23 @@
         <f t="shared" si="38"/>
         <v>90.625</v>
       </c>
-    </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S56" s="20">
+        <f t="shared" si="38"/>
+        <v>89.583299999999994</v>
+      </c>
+      <c r="T56" s="20"/>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B57" s="24">
-        <f t="shared" ref="B57:R57" si="39">AVERAGE(B48:B56)</f>
-        <v>80.936213251028803</v>
+        <f>AVERAGE(B48:B56)</f>
+        <v>81.083621450617272</v>
       </c>
       <c r="C57" s="25">
-        <f t="shared" si="39"/>
-        <v>86.516208641975297</v>
+        <f t="shared" ref="B57:S57" si="39">AVERAGE(C48:C56)</f>
+        <v>86.59336419753086</v>
       </c>
       <c r="D57" s="20">
         <f t="shared" si="39"/>
@@ -5254,125 +4647,222 @@
         <f t="shared" si="39"/>
         <v>84.259266666666662</v>
       </c>
-    </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="D58" s="33"/>
-      <c r="E58" s="33"/>
-      <c r="F58" s="33"/>
-      <c r="G58" s="33"/>
-      <c r="H58" s="33"/>
-      <c r="I58" s="33"/>
-      <c r="J58" s="33"/>
-      <c r="K58" s="33"/>
-      <c r="L58" s="33"/>
-      <c r="M58" s="33"/>
-      <c r="N58" s="33"/>
-      <c r="O58" s="33"/>
-      <c r="P58" s="33"/>
+      <c r="S57" s="20">
+        <f t="shared" si="39"/>
+        <v>83.294744444444461</v>
+      </c>
+      <c r="T57" s="20"/>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="D58" s="32"/>
+      <c r="E58" s="32"/>
+      <c r="F58" s="32"/>
+      <c r="G58" s="32"/>
+      <c r="H58" s="32"/>
+      <c r="I58" s="32"/>
+      <c r="J58" s="32"/>
+      <c r="K58" s="32"/>
+      <c r="L58" s="32"/>
+      <c r="M58" s="32"/>
+      <c r="N58" s="32"/>
+      <c r="O58" s="32"/>
+      <c r="P58" s="32"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="D47:J47"/>
-    <mergeCell ref="K18:M18"/>
-    <mergeCell ref="N18:Q18"/>
-    <mergeCell ref="N33:Q33"/>
-    <mergeCell ref="N47:Q47"/>
-    <mergeCell ref="L32:P32"/>
-    <mergeCell ref="L46:P46"/>
-    <mergeCell ref="D46:K46"/>
-    <mergeCell ref="D32:K32"/>
+  <mergeCells count="24">
+    <mergeCell ref="Q17:R17"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="N47:S47"/>
+    <mergeCell ref="N33:S33"/>
+    <mergeCell ref="N18:S18"/>
+    <mergeCell ref="N5:S5"/>
+    <mergeCell ref="Q32:S32"/>
+    <mergeCell ref="Q46:S46"/>
     <mergeCell ref="D5:J5"/>
     <mergeCell ref="D18:J18"/>
     <mergeCell ref="D33:J33"/>
-    <mergeCell ref="N5:Q5"/>
     <mergeCell ref="D4:K4"/>
     <mergeCell ref="L4:P4"/>
     <mergeCell ref="D17:K17"/>
     <mergeCell ref="L17:P17"/>
     <mergeCell ref="K5:M5"/>
+    <mergeCell ref="K33:M33"/>
+    <mergeCell ref="D47:J47"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="L32:P32"/>
+    <mergeCell ref="L46:P46"/>
+    <mergeCell ref="D46:K46"/>
+    <mergeCell ref="D32:K32"/>
     <mergeCell ref="K47:M47"/>
-    <mergeCell ref="K33:M33"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="D49:R49">
+  <conditionalFormatting sqref="T49">
+    <cfRule type="top10" dxfId="83" priority="109" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="82" priority="110" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T48">
+    <cfRule type="top10" dxfId="81" priority="107" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="80" priority="108" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T51">
+    <cfRule type="top10" dxfId="79" priority="105" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="78" priority="106" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T50">
+    <cfRule type="top10" dxfId="77" priority="103" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="76" priority="104" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T53">
+    <cfRule type="top10" dxfId="75" priority="101" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="74" priority="102" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T52">
+    <cfRule type="top10" dxfId="73" priority="99" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="72" priority="100" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T55">
+    <cfRule type="top10" dxfId="71" priority="97" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="70" priority="98" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T54">
+    <cfRule type="top10" dxfId="69" priority="95" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="68" priority="96" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T56">
+    <cfRule type="top10" dxfId="67" priority="91" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="66" priority="92" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T57">
+    <cfRule type="top10" dxfId="65" priority="67" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="64" priority="68" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T48:T56">
+    <cfRule type="top10" dxfId="63" priority="63" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="62" priority="64" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T35">
+    <cfRule type="top10" dxfId="61" priority="61" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="60" priority="62" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T34">
+    <cfRule type="top10" dxfId="59" priority="59" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="58" priority="60" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T37">
+    <cfRule type="top10" dxfId="57" priority="57" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="56" priority="58" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T36">
+    <cfRule type="top10" dxfId="55" priority="55" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="54" priority="56" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T39">
+    <cfRule type="top10" dxfId="53" priority="53" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="52" priority="54" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T38">
+    <cfRule type="top10" dxfId="51" priority="51" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="50" priority="52" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T41">
+    <cfRule type="top10" dxfId="49" priority="49" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="48" priority="50" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T40">
+    <cfRule type="top10" dxfId="47" priority="47" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="46" priority="48" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T42">
+    <cfRule type="top10" dxfId="45" priority="45" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="44" priority="46" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T43">
     <cfRule type="top10" dxfId="43" priority="43" bottom="1" rank="1"/>
     <cfRule type="top10" dxfId="42" priority="44" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D48:R48">
+  <conditionalFormatting sqref="T34:T42">
     <cfRule type="top10" dxfId="41" priority="41" bottom="1" rank="1"/>
     <cfRule type="top10" dxfId="40" priority="42" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D51:R51">
-    <cfRule type="top10" dxfId="39" priority="39" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="38" priority="40" rank="1"/>
+  <conditionalFormatting sqref="D35:S35">
+    <cfRule type="top10" dxfId="39" priority="111" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="38" priority="112" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D50:R50">
-    <cfRule type="top10" dxfId="37" priority="37" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="36" priority="38" rank="1"/>
+  <conditionalFormatting sqref="D34:S34">
+    <cfRule type="top10" dxfId="37" priority="113" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="36" priority="114" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D53:R53">
-    <cfRule type="top10" dxfId="35" priority="35" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="34" priority="36" rank="1"/>
+  <conditionalFormatting sqref="D37:S37">
+    <cfRule type="top10" dxfId="35" priority="115" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="34" priority="116" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D52:R52">
-    <cfRule type="top10" dxfId="33" priority="33" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="32" priority="34" rank="1"/>
+  <conditionalFormatting sqref="D36:S36">
+    <cfRule type="top10" dxfId="33" priority="117" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="32" priority="118" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D55:R55">
-    <cfRule type="top10" dxfId="31" priority="31" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="30" priority="32" rank="1"/>
+  <conditionalFormatting sqref="D39:S39">
+    <cfRule type="top10" dxfId="31" priority="119" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="30" priority="120" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D54:R54">
-    <cfRule type="top10" dxfId="29" priority="29" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="28" priority="30" rank="1"/>
+  <conditionalFormatting sqref="D38:S38">
+    <cfRule type="top10" dxfId="29" priority="121" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="28" priority="122" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D56:R56">
-    <cfRule type="top10" dxfId="25" priority="25" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="24" priority="26" rank="1"/>
+  <conditionalFormatting sqref="D41:S41">
+    <cfRule type="top10" dxfId="27" priority="123" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="26" priority="124" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D35:R35">
-    <cfRule type="top10" dxfId="23" priority="23" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="22" priority="24" rank="1"/>
+  <conditionalFormatting sqref="D40:S40">
+    <cfRule type="top10" dxfId="25" priority="125" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="24" priority="126" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D34:R34">
-    <cfRule type="top10" dxfId="21" priority="21" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="20" priority="22" rank="1"/>
+  <conditionalFormatting sqref="D42:S42">
+    <cfRule type="top10" dxfId="23" priority="127" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="22" priority="128" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D37:R37">
-    <cfRule type="top10" dxfId="19" priority="19" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="18" priority="20" rank="1"/>
+  <conditionalFormatting sqref="D43:S43">
+    <cfRule type="top10" dxfId="21" priority="129" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="20" priority="130" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D36:R36">
-    <cfRule type="top10" dxfId="17" priority="17" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="16" priority="18" rank="1"/>
+  <conditionalFormatting sqref="D49:S49">
+    <cfRule type="top10" dxfId="19" priority="131" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="18" priority="132" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D39:R39">
-    <cfRule type="top10" dxfId="15" priority="15" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="14" priority="16" rank="1"/>
+  <conditionalFormatting sqref="D48:S48">
+    <cfRule type="top10" dxfId="17" priority="133" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="16" priority="134" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D38:R38">
-    <cfRule type="top10" dxfId="13" priority="13" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="12" priority="14" rank="1"/>
+  <conditionalFormatting sqref="D51:S51">
+    <cfRule type="top10" dxfId="15" priority="135" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="14" priority="136" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D41:R41">
-    <cfRule type="top10" dxfId="11" priority="11" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="10" priority="12" rank="1"/>
+  <conditionalFormatting sqref="D50:S50">
+    <cfRule type="top10" dxfId="13" priority="137" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="12" priority="138" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D40:R40">
-    <cfRule type="top10" dxfId="9" priority="9" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="8" priority="10" rank="1"/>
+  <conditionalFormatting sqref="D53:S53">
+    <cfRule type="top10" dxfId="11" priority="139" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="10" priority="140" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D42:R42">
-    <cfRule type="top10" dxfId="5" priority="5" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="4" priority="6" rank="1"/>
+  <conditionalFormatting sqref="D52:S52">
+    <cfRule type="top10" dxfId="9" priority="141" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="8" priority="142" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D43:R43">
-    <cfRule type="top10" dxfId="3" priority="3" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="2" priority="4" rank="1"/>
+  <conditionalFormatting sqref="D55:S55">
+    <cfRule type="top10" dxfId="7" priority="143" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="6" priority="144" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D57:R57">
-    <cfRule type="top10" dxfId="1" priority="1" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="0" priority="2" rank="1"/>
+  <conditionalFormatting sqref="D54:S54">
+    <cfRule type="top10" dxfId="5" priority="145" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="4" priority="146" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D56:S56">
+    <cfRule type="top10" dxfId="3" priority="147" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="2" priority="148" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D57:S57">
+    <cfRule type="top10" dxfId="1" priority="149" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="0" priority="150" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Continue test on dataset 2a
</commit_message>
<xml_diff>
--- a/Saved model/Saved Results.xlsx
+++ b/Saved model/Saved Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\albi2\Documents\GitHub\Variational-Autoencoder-for-EEG-analysis\Saved model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{456556E9-1F8C-4ECB-A0C5-01B07BD7A8CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E9645DE-88EB-4DF7-8D1A-B165E00DF04E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1479,7 +1479,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:AC60"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
@@ -5970,8 +5970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9569107-D6A2-48F5-A7AB-646FE6B45B23}">
   <dimension ref="A2:AC60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G62" sqref="G62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6058,7 +6058,7 @@
       </c>
       <c r="B6" s="2">
         <f>AVERAGE(D6:BB6)</f>
-        <v>0.83680550000000009</v>
+        <v>0.84461800000000009</v>
       </c>
       <c r="C6" s="4">
         <f t="shared" ref="C6:C7" si="0">MAX(D6:BB6)</f>
@@ -6070,8 +6070,12 @@
       <c r="E6" s="3">
         <v>0.85763900000000004</v>
       </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
+      <c r="F6" s="3">
+        <v>0.84722200000000003</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0.85763900000000004</v>
+      </c>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
     </row>
@@ -6081,11 +6085,11 @@
       </c>
       <c r="B7" s="7">
         <f t="shared" ref="B7:B13" si="1">AVERAGE(D7:BB7)</f>
-        <v>0.72222200000000003</v>
+        <v>0.73611099999999996</v>
       </c>
       <c r="C7" s="9">
         <f t="shared" si="0"/>
-        <v>0.72222200000000003</v>
+        <v>0.77083299999999999</v>
       </c>
       <c r="D7" s="8">
         <v>0.72222200000000003</v>
@@ -6093,8 +6097,12 @@
       <c r="E7" s="8">
         <v>0.72222200000000003</v>
       </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
+      <c r="F7" s="8">
+        <v>0.77083299999999999</v>
+      </c>
+      <c r="G7" s="8">
+        <v>0.72916700000000001</v>
+      </c>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
     </row>
@@ -6104,11 +6112,11 @@
       </c>
       <c r="B8" s="7">
         <f t="shared" si="1"/>
-        <v>0.84722249999999999</v>
+        <v>0.87239600000000006</v>
       </c>
       <c r="C8" s="9">
         <f>MAX(D8:BB8)</f>
-        <v>0.88541700000000001</v>
+        <v>0.89930600000000005</v>
       </c>
       <c r="D8" s="8">
         <v>0.80902799999999997</v>
@@ -6116,8 +6124,12 @@
       <c r="E8" s="8">
         <v>0.88541700000000001</v>
       </c>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
+      <c r="F8" s="8">
+        <v>0.89583299999999999</v>
+      </c>
+      <c r="G8" s="8">
+        <v>0.89930600000000005</v>
+      </c>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
     </row>
@@ -6127,7 +6139,7 @@
       </c>
       <c r="B9" s="7">
         <f t="shared" si="1"/>
-        <v>0.74739599999999995</v>
+        <v>0.73828125</v>
       </c>
       <c r="C9" s="9">
         <f t="shared" ref="C9:C14" si="2">MAX(D9:BB9)</f>
@@ -6139,8 +6151,12 @@
       <c r="E9" s="8">
         <v>0.78125</v>
       </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
+      <c r="F9" s="8">
+        <v>0.734375</v>
+      </c>
+      <c r="G9" s="8">
+        <v>0.72395799999999999</v>
+      </c>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
     </row>
@@ -6150,11 +6166,11 @@
       </c>
       <c r="B10" s="7">
         <f t="shared" si="1"/>
-        <v>0.82986099999999996</v>
+        <v>0.82899299999999998</v>
       </c>
       <c r="C10" s="9">
         <f t="shared" si="2"/>
-        <v>0.83333299999999999</v>
+        <v>0.84722200000000003</v>
       </c>
       <c r="D10" s="8">
         <v>0.83333299999999999</v>
@@ -6162,8 +6178,12 @@
       <c r="E10" s="8">
         <v>0.82638900000000004</v>
       </c>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
+      <c r="F10" s="8">
+        <v>0.84722200000000003</v>
+      </c>
+      <c r="G10" s="8">
+        <v>0.80902799999999997</v>
+      </c>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
     </row>
@@ -6173,11 +6193,11 @@
       </c>
       <c r="B11" s="7">
         <f t="shared" si="1"/>
-        <v>0.80729200000000001</v>
+        <v>0.82986150000000003</v>
       </c>
       <c r="C11" s="9">
         <f t="shared" si="2"/>
-        <v>0.85416700000000001</v>
+        <v>0.86805600000000005</v>
       </c>
       <c r="D11" s="8">
         <v>0.76041700000000001</v>
@@ -6185,8 +6205,12 @@
       <c r="E11" s="8">
         <v>0.85416700000000001</v>
       </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
+      <c r="F11" s="8">
+        <v>0.86805600000000005</v>
+      </c>
+      <c r="G11" s="8">
+        <v>0.83680600000000005</v>
+      </c>
       <c r="H11" s="8"/>
       <c r="I11" s="8"/>
     </row>
@@ -6196,7 +6220,7 @@
       </c>
       <c r="B12" s="7">
         <f t="shared" si="1"/>
-        <v>0.86979200000000001</v>
+        <v>0.86805575000000001</v>
       </c>
       <c r="C12" s="9">
         <f t="shared" si="2"/>
@@ -6208,8 +6232,12 @@
       <c r="E12" s="8">
         <v>0.88541700000000001</v>
       </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
+      <c r="F12" s="8">
+        <v>0.86458299999999999</v>
+      </c>
+      <c r="G12" s="8">
+        <v>0.86805600000000005</v>
+      </c>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
     </row>
@@ -6219,7 +6247,7 @@
       </c>
       <c r="B13" s="7">
         <f t="shared" si="1"/>
-        <v>0.85763900000000004</v>
+        <v>0.86371550000000008</v>
       </c>
       <c r="C13" s="9">
         <f t="shared" si="2"/>
@@ -6231,8 +6259,12 @@
       <c r="E13" s="8">
         <v>0.88541700000000001</v>
       </c>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
+      <c r="F13" s="8">
+        <v>0.86805600000000005</v>
+      </c>
+      <c r="G13" s="8">
+        <v>0.87152799999999997</v>
+      </c>
       <c r="H13" s="8"/>
       <c r="I13" s="8"/>
     </row>
@@ -6242,7 +6274,7 @@
       </c>
       <c r="B14" s="11">
         <f>AVERAGE(D14:BB14)</f>
-        <v>0.89236099999999996</v>
+        <v>0.90364575000000003</v>
       </c>
       <c r="C14" s="30">
         <f t="shared" si="2"/>
@@ -6254,8 +6286,12 @@
       <c r="E14" s="12">
         <v>0.92708299999999999</v>
       </c>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
+      <c r="F14" s="12">
+        <v>0.92708299999999999</v>
+      </c>
+      <c r="G14" s="12">
+        <v>0.90277799999999997</v>
+      </c>
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
     </row>
@@ -6263,11 +6299,11 @@
       <c r="A15" s="8"/>
       <c r="B15" s="13">
         <f t="shared" ref="B15:C15" si="3">AVERAGE(B6:B14)</f>
-        <v>0.8233990000000001</v>
+        <v>0.83174197222222224</v>
       </c>
       <c r="C15" s="15">
         <f t="shared" si="3"/>
-        <v>0.84799388888888894</v>
+        <v>0.85802477777777786</v>
       </c>
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
@@ -6389,7 +6425,7 @@
       </c>
       <c r="B19" s="2">
         <f>AVERAGE(D19:BB19)</f>
-        <v>0.85243050000000009</v>
+        <v>0.84375</v>
       </c>
       <c r="C19" s="4">
         <f t="shared" ref="C19:C20" si="4">MAX(D19:BB19)</f>
@@ -6401,8 +6437,12 @@
       <c r="E19" s="8">
         <v>0.85763900000000004</v>
       </c>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
+      <c r="F19" s="8">
+        <v>0.84375</v>
+      </c>
+      <c r="G19" s="8">
+        <v>0.82638900000000004</v>
+      </c>
       <c r="H19" s="8"/>
       <c r="I19" s="8"/>
       <c r="J19" s="8"/>
@@ -6432,7 +6472,7 @@
       </c>
       <c r="C20" s="9">
         <f t="shared" si="4"/>
-        <v>0.76041700000000001</v>
+        <v>0.77083299999999999</v>
       </c>
       <c r="D20" s="8">
         <v>0.76041700000000001</v>
@@ -6440,8 +6480,12 @@
       <c r="E20" s="8">
         <v>0.72222200000000003</v>
       </c>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
+      <c r="F20" s="8">
+        <v>0.77083299999999999</v>
+      </c>
+      <c r="G20" s="8">
+        <v>0.71180600000000005</v>
+      </c>
       <c r="H20" s="8"/>
       <c r="I20" s="8"/>
       <c r="J20" s="8"/>
@@ -6467,7 +6511,7 @@
       </c>
       <c r="B21" s="7">
         <f t="shared" si="5"/>
-        <v>0.88368049999999998</v>
+        <v>0.88194450000000002</v>
       </c>
       <c r="C21" s="9">
         <f>MAX(D21:BB21)</f>
@@ -6479,8 +6523,12 @@
       <c r="E21" s="8">
         <v>0.88541700000000001</v>
       </c>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
+      <c r="F21" s="8">
+        <v>0.88541700000000001</v>
+      </c>
+      <c r="G21" s="8">
+        <v>0.875</v>
+      </c>
       <c r="H21" s="8"/>
       <c r="I21" s="8"/>
       <c r="J21" s="8"/>
@@ -6506,7 +6554,7 @@
       </c>
       <c r="B22" s="7">
         <f t="shared" si="5"/>
-        <v>0.77864599999999995</v>
+        <v>0.76432299999999997</v>
       </c>
       <c r="C22" s="9">
         <f t="shared" ref="C22:C27" si="6">MAX(D22:BB22)</f>
@@ -6518,8 +6566,12 @@
       <c r="E22" s="8">
         <v>0.78125</v>
       </c>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
+      <c r="F22" s="8">
+        <v>0.77083299999999999</v>
+      </c>
+      <c r="G22" s="8">
+        <v>0.72916700000000001</v>
+      </c>
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
@@ -6545,7 +6597,7 @@
       </c>
       <c r="B23" s="7">
         <f t="shared" si="5"/>
-        <v>0.83333349999999995</v>
+        <v>0.82899299999999998</v>
       </c>
       <c r="C23" s="9">
         <f t="shared" si="6"/>
@@ -6557,8 +6609,12 @@
       <c r="E23" s="8">
         <v>0.82638900000000004</v>
       </c>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
+      <c r="F23" s="8">
+        <v>0.83333299999999999</v>
+      </c>
+      <c r="G23" s="8">
+        <v>0.81597200000000003</v>
+      </c>
       <c r="H23" s="8"/>
       <c r="I23" s="8"/>
       <c r="J23" s="8"/>
@@ -6584,7 +6640,7 @@
       </c>
       <c r="B24" s="7">
         <f t="shared" si="5"/>
-        <v>0.84548650000000003</v>
+        <v>0.84461825000000001</v>
       </c>
       <c r="C24" s="9">
         <f t="shared" si="6"/>
@@ -6596,8 +6652,12 @@
       <c r="E24" s="8">
         <v>0.85416700000000001</v>
       </c>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
+      <c r="F24" s="8">
+        <v>0.84722200000000003</v>
+      </c>
+      <c r="G24" s="8">
+        <v>0.84027799999999997</v>
+      </c>
       <c r="H24" s="8"/>
       <c r="I24" s="8"/>
       <c r="J24" s="8"/>
@@ -6623,7 +6683,7 @@
       </c>
       <c r="B25" s="7">
         <f t="shared" si="5"/>
-        <v>0.88715300000000008</v>
+        <v>0.87934050000000008</v>
       </c>
       <c r="C25" s="9">
         <f t="shared" si="6"/>
@@ -6635,8 +6695,12 @@
       <c r="E25" s="8">
         <v>0.88541700000000001</v>
       </c>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
+      <c r="F25" s="8">
+        <v>0.86805600000000005</v>
+      </c>
+      <c r="G25" s="8">
+        <v>0.875</v>
+      </c>
       <c r="H25" s="8"/>
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
@@ -6662,11 +6726,11 @@
       </c>
       <c r="B26" s="7">
         <f t="shared" si="5"/>
-        <v>0.88541700000000001</v>
+        <v>0.8836807499999999</v>
       </c>
       <c r="C26" s="9">
         <f t="shared" si="6"/>
-        <v>0.88541700000000001</v>
+        <v>0.89236099999999996</v>
       </c>
       <c r="D26" s="8">
         <v>0.88541700000000001</v>
@@ -6674,8 +6738,12 @@
       <c r="E26" s="8">
         <v>0.88541700000000001</v>
       </c>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
+      <c r="F26" s="8">
+        <v>0.87152799999999997</v>
+      </c>
+      <c r="G26" s="8">
+        <v>0.89236099999999996</v>
+      </c>
       <c r="H26" s="8"/>
       <c r="I26" s="8"/>
       <c r="J26" s="8"/>
@@ -6701,7 +6769,7 @@
       </c>
       <c r="B27" s="11">
         <f>AVERAGE(D27:BB27)</f>
-        <v>0.93576349999999997</v>
+        <v>0.92187474999999997</v>
       </c>
       <c r="C27" s="30">
         <f t="shared" si="6"/>
@@ -6713,8 +6781,12 @@
       <c r="E27" s="8">
         <v>0.92708299999999999</v>
       </c>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
+      <c r="F27" s="8">
+        <v>0.91319399999999995</v>
+      </c>
+      <c r="G27" s="8">
+        <v>0.90277799999999997</v>
+      </c>
       <c r="H27" s="8"/>
       <c r="I27" s="8"/>
       <c r="J27" s="8"/>
@@ -6740,11 +6812,11 @@
       </c>
       <c r="B28" s="13">
         <f t="shared" ref="B28:C28" si="7">AVERAGE(B19:B27)</f>
-        <v>0.84924777777777782</v>
+        <v>0.8433160277777777</v>
       </c>
       <c r="C28" s="15">
         <f t="shared" si="7"/>
-        <v>0.85532422222222226</v>
+        <v>0.85725311111111102</v>
       </c>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
@@ -6847,7 +6919,7 @@
       </c>
       <c r="B34" s="16">
         <f>B6 * 100</f>
-        <v>83.680550000000011</v>
+        <v>84.461800000000011</v>
       </c>
       <c r="C34" s="17">
         <f t="shared" ref="C34:J34" si="8">C6 * 100</f>
@@ -6863,11 +6935,11 @@
       </c>
       <c r="F34" s="19">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>84.722200000000001</v>
       </c>
       <c r="G34" s="19">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>85.763900000000007</v>
       </c>
       <c r="H34" s="19">
         <f t="shared" si="8"/>
@@ -6956,11 +7028,11 @@
       </c>
       <c r="B35" s="18">
         <f t="shared" ref="B35:L42" si="10">B7 * 100</f>
-        <v>72.222200000000001</v>
+        <v>73.611099999999993</v>
       </c>
       <c r="C35" s="20">
         <f t="shared" si="10"/>
-        <v>72.222200000000001</v>
+        <v>77.083299999999994</v>
       </c>
       <c r="D35" s="19">
         <f t="shared" si="10"/>
@@ -6972,11 +7044,11 @@
       </c>
       <c r="F35" s="19">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>77.083299999999994</v>
       </c>
       <c r="G35" s="19">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>72.916700000000006</v>
       </c>
       <c r="H35" s="19">
         <f t="shared" si="10"/>
@@ -7065,11 +7137,11 @@
       </c>
       <c r="B36" s="18">
         <f t="shared" si="10"/>
-        <v>84.722250000000003</v>
+        <v>87.23960000000001</v>
       </c>
       <c r="C36" s="20">
         <f t="shared" si="10"/>
-        <v>88.541700000000006</v>
+        <v>89.930599999999998</v>
       </c>
       <c r="D36" s="19">
         <f t="shared" si="10"/>
@@ -7081,11 +7153,11 @@
       </c>
       <c r="F36" s="19">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>89.583299999999994</v>
       </c>
       <c r="G36" s="19">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>89.930599999999998</v>
       </c>
       <c r="H36" s="19">
         <f t="shared" si="10"/>
@@ -7174,7 +7246,7 @@
       </c>
       <c r="B37" s="18">
         <f t="shared" si="10"/>
-        <v>74.739599999999996</v>
+        <v>73.828125</v>
       </c>
       <c r="C37" s="20">
         <f t="shared" si="10"/>
@@ -7190,11 +7262,11 @@
       </c>
       <c r="F37" s="19">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>73.4375</v>
       </c>
       <c r="G37" s="19">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>72.395799999999994</v>
       </c>
       <c r="H37" s="19">
         <f t="shared" si="10"/>
@@ -7283,11 +7355,11 @@
       </c>
       <c r="B38" s="18">
         <f t="shared" si="10"/>
-        <v>82.986099999999993</v>
+        <v>82.899299999999997</v>
       </c>
       <c r="C38" s="20">
         <f t="shared" si="10"/>
-        <v>83.333299999999994</v>
+        <v>84.722200000000001</v>
       </c>
       <c r="D38" s="19">
         <f t="shared" si="10"/>
@@ -7299,11 +7371,11 @@
       </c>
       <c r="F38" s="19">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>84.722200000000001</v>
       </c>
       <c r="G38" s="19">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>80.902799999999999</v>
       </c>
       <c r="H38" s="19">
         <f t="shared" si="10"/>
@@ -7392,11 +7464,11 @@
       </c>
       <c r="B39" s="18">
         <f t="shared" si="10"/>
-        <v>80.729200000000006</v>
+        <v>82.986150000000009</v>
       </c>
       <c r="C39" s="20">
         <f t="shared" si="10"/>
-        <v>85.416700000000006</v>
+        <v>86.805599999999998</v>
       </c>
       <c r="D39" s="19">
         <f t="shared" si="10"/>
@@ -7408,11 +7480,11 @@
       </c>
       <c r="F39" s="19">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>86.805599999999998</v>
       </c>
       <c r="G39" s="19">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>83.680599999999998</v>
       </c>
       <c r="H39" s="19">
         <f t="shared" si="10"/>
@@ -7501,7 +7573,7 @@
       </c>
       <c r="B40" s="18">
         <f t="shared" si="10"/>
-        <v>86.979200000000006</v>
+        <v>86.805575000000005</v>
       </c>
       <c r="C40" s="20">
         <f t="shared" si="10"/>
@@ -7517,11 +7589,11 @@
       </c>
       <c r="F40" s="19">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>86.458299999999994</v>
       </c>
       <c r="G40" s="19">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>86.805599999999998</v>
       </c>
       <c r="H40" s="19">
         <f t="shared" si="10"/>
@@ -7610,7 +7682,7 @@
       </c>
       <c r="B41" s="18">
         <f t="shared" si="10"/>
-        <v>85.763900000000007</v>
+        <v>86.371550000000013</v>
       </c>
       <c r="C41" s="20">
         <f t="shared" si="10"/>
@@ -7626,11 +7698,11 @@
       </c>
       <c r="F41" s="19">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>86.805599999999998</v>
       </c>
       <c r="G41" s="19">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>87.152799999999999</v>
       </c>
       <c r="H41" s="19">
         <f t="shared" si="10"/>
@@ -7719,7 +7791,7 @@
       </c>
       <c r="B42" s="21">
         <f t="shared" si="10"/>
-        <v>89.236099999999993</v>
+        <v>90.364575000000002</v>
       </c>
       <c r="C42" s="22">
         <f t="shared" si="10"/>
@@ -7735,11 +7807,11 @@
       </c>
       <c r="F42" s="19">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>92.708299999999994</v>
       </c>
       <c r="G42" s="19">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>90.277799999999999</v>
       </c>
       <c r="H42" s="19">
         <f t="shared" si="10"/>
@@ -7828,11 +7900,11 @@
       </c>
       <c r="B43" s="23">
         <f t="shared" ref="B43:Y43" si="11">AVERAGE(B34:B42)</f>
-        <v>82.3399</v>
+        <v>83.174197222222219</v>
       </c>
       <c r="C43" s="24">
         <f t="shared" si="11"/>
-        <v>84.799388888888899</v>
+        <v>85.802477777777767</v>
       </c>
       <c r="D43" s="19">
         <f t="shared" si="11"/>
@@ -7844,11 +7916,11 @@
       </c>
       <c r="F43" s="19">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>84.702922222222227</v>
       </c>
       <c r="G43" s="19">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>83.314066666666662</v>
       </c>
       <c r="H43" s="19">
         <f t="shared" si="11"/>
@@ -8031,7 +8103,7 @@
       </c>
       <c r="B48" s="16">
         <f>B19 * 100</f>
-        <v>85.243050000000011</v>
+        <v>84.375</v>
       </c>
       <c r="C48" s="17">
         <f t="shared" ref="C48:K48" si="12">C19 * 100</f>
@@ -8047,11 +8119,11 @@
       </c>
       <c r="F48" s="19">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>84.375</v>
       </c>
       <c r="G48" s="19">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>82.638900000000007</v>
       </c>
       <c r="H48" s="19">
         <f t="shared" si="12"/>
@@ -8144,23 +8216,23 @@
       </c>
       <c r="C49" s="20">
         <f t="shared" si="14"/>
+        <v>77.083299999999994</v>
+      </c>
+      <c r="D49" s="19">
+        <f t="shared" si="14"/>
         <v>76.041700000000006</v>
       </c>
-      <c r="D49" s="19">
-        <f t="shared" si="14"/>
-        <v>76.041700000000006</v>
-      </c>
       <c r="E49" s="19">
         <f t="shared" si="14"/>
         <v>72.222200000000001</v>
       </c>
       <c r="F49" s="19">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>77.083299999999994</v>
       </c>
       <c r="G49" s="19">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>71.180599999999998</v>
       </c>
       <c r="H49" s="19">
         <f t="shared" si="14"/>
@@ -8249,7 +8321,7 @@
       </c>
       <c r="B50" s="18">
         <f t="shared" si="14"/>
-        <v>88.368049999999997</v>
+        <v>88.194450000000003</v>
       </c>
       <c r="C50" s="20">
         <f t="shared" si="14"/>
@@ -8265,11 +8337,11 @@
       </c>
       <c r="F50" s="19">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>88.541700000000006</v>
       </c>
       <c r="G50" s="19">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>87.5</v>
       </c>
       <c r="H50" s="19">
         <f t="shared" si="14"/>
@@ -8358,7 +8430,7 @@
       </c>
       <c r="B51" s="18">
         <f t="shared" si="14"/>
-        <v>77.864599999999996</v>
+        <v>76.432299999999998</v>
       </c>
       <c r="C51" s="20">
         <f t="shared" si="14"/>
@@ -8374,11 +8446,11 @@
       </c>
       <c r="F51" s="19">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>77.083299999999994</v>
       </c>
       <c r="G51" s="19">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>72.916700000000006</v>
       </c>
       <c r="H51" s="19">
         <f t="shared" si="14"/>
@@ -8467,7 +8539,7 @@
       </c>
       <c r="B52" s="18">
         <f t="shared" si="14"/>
-        <v>83.333349999999996</v>
+        <v>82.899299999999997</v>
       </c>
       <c r="C52" s="20">
         <f t="shared" si="14"/>
@@ -8483,11 +8555,11 @@
       </c>
       <c r="F52" s="19">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>83.333299999999994</v>
       </c>
       <c r="G52" s="19">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>81.597200000000001</v>
       </c>
       <c r="H52" s="19">
         <f t="shared" si="14"/>
@@ -8576,7 +8648,7 @@
       </c>
       <c r="B53" s="18">
         <f t="shared" si="14"/>
-        <v>84.548650000000009</v>
+        <v>84.461825000000005</v>
       </c>
       <c r="C53" s="20">
         <f t="shared" si="14"/>
@@ -8592,11 +8664,11 @@
       </c>
       <c r="F53" s="19">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>84.722200000000001</v>
       </c>
       <c r="G53" s="19">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>84.027799999999999</v>
       </c>
       <c r="H53" s="19">
         <f t="shared" si="14"/>
@@ -8685,7 +8757,7 @@
       </c>
       <c r="B54" s="18">
         <f t="shared" si="14"/>
-        <v>88.715300000000013</v>
+        <v>87.934050000000013</v>
       </c>
       <c r="C54" s="20">
         <f t="shared" si="14"/>
@@ -8701,11 +8773,11 @@
       </c>
       <c r="F54" s="19">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>86.805599999999998</v>
       </c>
       <c r="G54" s="19">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>87.5</v>
       </c>
       <c r="H54" s="19">
         <f t="shared" si="14"/>
@@ -8794,27 +8866,27 @@
       </c>
       <c r="B55" s="18">
         <f t="shared" si="14"/>
+        <v>88.36807499999999</v>
+      </c>
+      <c r="C55" s="20">
+        <f t="shared" si="14"/>
+        <v>89.236099999999993</v>
+      </c>
+      <c r="D55" s="19">
+        <f t="shared" si="14"/>
         <v>88.541700000000006</v>
       </c>
-      <c r="C55" s="20">
+      <c r="E55" s="19">
         <f t="shared" si="14"/>
         <v>88.541700000000006</v>
       </c>
-      <c r="D55" s="19">
-        <f t="shared" si="14"/>
-        <v>88.541700000000006</v>
-      </c>
-      <c r="E55" s="19">
-        <f t="shared" si="14"/>
-        <v>88.541700000000006</v>
-      </c>
       <c r="F55" s="19">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>87.152799999999999</v>
       </c>
       <c r="G55" s="19">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>89.236099999999993</v>
       </c>
       <c r="H55" s="19">
         <f t="shared" si="14"/>
@@ -8903,7 +8975,7 @@
       </c>
       <c r="B56" s="21">
         <f t="shared" si="14"/>
-        <v>93.576349999999991</v>
+        <v>92.187474999999992</v>
       </c>
       <c r="C56" s="22">
         <f t="shared" si="14"/>
@@ -8919,11 +8991,11 @@
       </c>
       <c r="F56" s="19">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>91.319400000000002</v>
       </c>
       <c r="G56" s="19">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>90.277799999999999</v>
       </c>
       <c r="H56" s="19">
         <f t="shared" si="14"/>
@@ -9012,11 +9084,11 @@
       </c>
       <c r="B57" s="23">
         <f>AVERAGE(B48:B56)</f>
-        <v>84.924777777777791</v>
+        <v>84.331602777777775</v>
       </c>
       <c r="C57" s="24">
         <f t="shared" ref="C57:AA57" si="15">AVERAGE(C48:C56)</f>
-        <v>85.532422222222223</v>
+        <v>85.725311111111111</v>
       </c>
       <c r="D57" s="19">
         <f t="shared" si="15"/>
@@ -9028,11 +9100,11 @@
       </c>
       <c r="F57" s="19">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>84.490733333333324</v>
       </c>
       <c r="G57" s="19">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>82.986122222222221</v>
       </c>
       <c r="H57" s="19">
         <f t="shared" si="15"/>

</xml_diff>